<commit_message>
Kosten und Erloesplaene angepasst an risikofreie Foerderung.
</commit_message>
<xml_diff>
--- a/Produktionsförderung/Anlage_6_Vorlage_Erloesvorschau_GBW.xlsx
+++ b/Produktionsförderung/Anlage_6_Vorlage_Erloesvorschau_GBW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ScrewDriversMFG\Produktionsförderung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1DF34-4028-466A-817C-83C338491221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8921CF1C-A9AA-4241-AFFC-CCCE64EA362A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="1095" windowWidth="52755" windowHeight="27525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produktname_Erlösvorschau" sheetId="1" r:id="rId1"/>
@@ -792,6 +792,21 @@
     <xf numFmtId="164" fontId="23" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="23" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -806,21 +821,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:BA995"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="18">
@@ -1246,78 +1246,78 @@
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="59"/>
+      <c r="B5" s="64"/>
       <c r="C5" s="41">
+        <v>45870</v>
+      </c>
+      <c r="D5" s="41">
+        <v>45901</v>
+      </c>
+      <c r="E5" s="41">
+        <v>45931</v>
+      </c>
+      <c r="F5" s="41">
+        <v>45962</v>
+      </c>
+      <c r="G5" s="41">
+        <v>45992</v>
+      </c>
+      <c r="H5" s="41">
+        <v>46023</v>
+      </c>
+      <c r="I5" s="41">
         <v>46054</v>
       </c>
-      <c r="D5" s="41">
+      <c r="J5" s="41">
         <v>46082</v>
       </c>
-      <c r="E5" s="41">
+      <c r="K5" s="41">
         <v>46113</v>
       </c>
-      <c r="F5" s="41">
+      <c r="L5" s="41">
         <v>46143</v>
       </c>
-      <c r="G5" s="41">
+      <c r="M5" s="41">
         <v>46174</v>
       </c>
-      <c r="H5" s="41">
+      <c r="N5" s="41">
         <v>46204</v>
       </c>
-      <c r="I5" s="41">
+      <c r="O5" s="41">
         <v>46235</v>
       </c>
-      <c r="J5" s="41">
+      <c r="P5" s="41">
         <v>46266</v>
       </c>
-      <c r="K5" s="41">
+      <c r="Q5" s="41">
         <v>46296</v>
       </c>
-      <c r="L5" s="41">
+      <c r="R5" s="41">
         <v>46327</v>
       </c>
-      <c r="M5" s="41">
+      <c r="S5" s="41">
         <v>46357</v>
       </c>
-      <c r="N5" s="41">
+      <c r="T5" s="41">
         <v>46388</v>
       </c>
-      <c r="O5" s="41">
+      <c r="U5" s="41">
         <v>46419</v>
       </c>
-      <c r="P5" s="41">
+      <c r="V5" s="41">
         <v>46447</v>
       </c>
-      <c r="Q5" s="41">
+      <c r="W5" s="41">
         <v>46478</v>
       </c>
-      <c r="R5" s="41">
+      <c r="X5" s="41">
         <v>46508</v>
       </c>
-      <c r="S5" s="41">
+      <c r="Y5" s="41">
         <v>46539</v>
       </c>
-      <c r="T5" s="41">
+      <c r="Z5" s="41">
         <v>46569</v>
-      </c>
-      <c r="U5" s="41">
-        <v>46600</v>
-      </c>
-      <c r="V5" s="41">
-        <v>46631</v>
-      </c>
-      <c r="W5" s="41">
-        <v>46661</v>
-      </c>
-      <c r="X5" s="41">
-        <v>46692</v>
-      </c>
-      <c r="Y5" s="41">
-        <v>46722</v>
-      </c>
-      <c r="Z5" s="41">
-        <v>46753</v>
       </c>
       <c r="AA5" s="21" t="s">
         <v>1</v>
@@ -1338,30 +1338,30 @@
       <c r="B6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="55"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
+      <c r="Z6" s="60"/>
       <c r="AA6" s="23"/>
       <c r="AB6" s="42" t="s">
         <v>42</v>
@@ -1448,7 +1448,7 @@
       <c r="Z7" s="25">
         <v>7.99</v>
       </c>
-      <c r="AA7" s="56"/>
+      <c r="AA7" s="61"/>
       <c r="AB7" s="42" t="s">
         <v>43</v>
       </c>
@@ -1534,7 +1534,7 @@
       <c r="Z8" s="12">
         <v>10</v>
       </c>
-      <c r="AA8" s="57"/>
+      <c r="AA8" s="62"/>
       <c r="AB8" s="42" t="s">
         <v>44</v>
       </c>
@@ -1643,7 +1643,7 @@
         <f t="shared" si="0"/>
         <v>7.1909999999999998</v>
       </c>
-      <c r="AA9" s="57"/>
+      <c r="AA9" s="62"/>
       <c r="AB9" s="42" t="s">
         <v>45</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="Z10" s="26">
         <v>30</v>
       </c>
-      <c r="AA10" s="57"/>
+      <c r="AA10" s="62"/>
       <c r="AB10" s="42" t="s">
         <v>46</v>
       </c>
@@ -1837,7 +1837,7 @@
         <f t="shared" si="1"/>
         <v>5.0336999999999996</v>
       </c>
-      <c r="AA11" s="57"/>
+      <c r="AA11" s="62"/>
       <c r="AB11" s="42"/>
     </row>
     <row r="12" spans="1:31" ht="15" x14ac:dyDescent="0.3">
@@ -1846,28 +1846,28 @@
         <v>7</v>
       </c>
       <c r="C12" s="30">
-        <f>((AD5)*10)*5</f>
-        <v>30000</v>
+        <f>((AD5)*10)*4</f>
+        <v>24000</v>
       </c>
       <c r="D12" s="30">
-        <f>((AD6)*10)*5</f>
-        <v>4500</v>
+        <f>((AD6)*10)*4</f>
+        <v>3600</v>
       </c>
       <c r="E12" s="14">
-        <f>((AD7)*10)*5</f>
-        <v>1350</v>
+        <f>((AD7)*10)*4</f>
+        <v>1080</v>
       </c>
       <c r="F12" s="30">
-        <f>((AD8)*10)*5</f>
-        <v>650</v>
+        <f>((AD8)*10)*4</f>
+        <v>520</v>
       </c>
       <c r="G12" s="30">
-        <f>((AD9)*10)*5+(AD5*10)</f>
-        <v>6350</v>
+        <f>((AD9)*10)*4+(AD5*10)</f>
+        <v>6280</v>
       </c>
       <c r="H12" s="14">
-        <f>((AD10)*10)*5+((AD6)*10)</f>
-        <v>1050</v>
+        <f>((AD10)*10)*4+((AD6)*10)</f>
+        <v>1020</v>
       </c>
       <c r="I12" s="30">
         <f>((AD7)*10)</f>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="AA12" s="31">
         <f t="shared" ref="AA12:AA13" si="2">SUM(C12:Z12)</f>
-        <v>73900</v>
+        <v>66500</v>
       </c>
       <c r="AB12" s="42"/>
     </row>
@@ -1954,27 +1954,27 @@
       </c>
       <c r="C13" s="15">
         <f t="shared" ref="C13:Z13" si="3">C11*C12</f>
-        <v>117453</v>
+        <v>93962.4</v>
       </c>
       <c r="D13" s="15">
         <f>D11*D12</f>
-        <v>22651.649999999998</v>
+        <v>18121.32</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="3"/>
-        <v>6795.4949999999999</v>
+        <v>5436.3959999999997</v>
       </c>
       <c r="F13" s="15">
         <f t="shared" si="3"/>
-        <v>2544.8150000000001</v>
+        <v>2035.8519999999999</v>
       </c>
       <c r="G13" s="15">
         <f t="shared" si="3"/>
-        <v>31963.994999999999</v>
+        <v>31611.635999999999</v>
       </c>
       <c r="H13" s="16">
         <f t="shared" si="3"/>
-        <v>5285.3849999999993</v>
+        <v>5134.3739999999998</v>
       </c>
       <c r="I13" s="15">
         <f t="shared" si="3"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="AA13" s="33">
         <f t="shared" si="2"/>
-        <v>319807.73999999993</v>
+        <v>289415.37799999991</v>
       </c>
       <c r="AB13" s="42" t="s">
         <v>47</v>
@@ -2064,30 +2064,30 @@
       <c r="B14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="61"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="61"/>
-      <c r="U14" s="61"/>
-      <c r="V14" s="61"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
+      <c r="U14" s="66"/>
+      <c r="V14" s="66"/>
+      <c r="W14" s="66"/>
+      <c r="X14" s="66"/>
+      <c r="Y14" s="66"/>
+      <c r="Z14" s="66"/>
       <c r="AA14" s="34"/>
       <c r="AB14" s="42" t="s">
         <v>48</v>
@@ -2174,7 +2174,7 @@
       <c r="Z15" s="25">
         <v>0.1</v>
       </c>
-      <c r="AA15" s="56"/>
+      <c r="AA15" s="61"/>
       <c r="AB15" s="42" t="s">
         <v>49</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="Z16" s="12">
         <v>0</v>
       </c>
-      <c r="AA16" s="57"/>
+      <c r="AA16" s="62"/>
       <c r="AB16" t="s">
         <v>50</v>
       </c>
@@ -2370,7 +2370,7 @@
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="AA17" s="57"/>
+      <c r="AA17" s="62"/>
       <c r="AB17" t="s">
         <v>51</v>
       </c>
@@ -2456,7 +2456,7 @@
       <c r="Z18" s="12">
         <v>0</v>
       </c>
-      <c r="AA18" s="57"/>
+      <c r="AA18" s="62"/>
       <c r="AB18" t="s">
         <v>52</v>
       </c>
@@ -2566,7 +2566,7 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
-      <c r="AA19" s="57"/>
+      <c r="AA19" s="62"/>
       <c r="AB19" t="s">
         <v>53</v>
       </c>
@@ -2780,30 +2780,30 @@
       <c r="B22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="61"/>
-      <c r="R22" s="61"/>
-      <c r="S22" s="61"/>
-      <c r="T22" s="61"/>
-      <c r="U22" s="61"/>
-      <c r="V22" s="61"/>
-      <c r="W22" s="61"/>
-      <c r="X22" s="61"/>
-      <c r="Y22" s="61"/>
-      <c r="Z22" s="61"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="66"/>
+      <c r="Y22" s="66"/>
+      <c r="Z22" s="66"/>
       <c r="AA22" s="34"/>
       <c r="AD22">
         <f t="shared" si="4"/>
@@ -2887,7 +2887,7 @@
       <c r="Z23" s="25">
         <v>2.99</v>
       </c>
-      <c r="AA23" s="56"/>
+      <c r="AA23" s="61"/>
       <c r="AD23">
         <f t="shared" si="4"/>
         <v>644</v>
@@ -2970,7 +2970,7 @@
       <c r="Z24" s="12">
         <v>0</v>
       </c>
-      <c r="AA24" s="57"/>
+      <c r="AA24" s="62"/>
       <c r="AD24">
         <f t="shared" si="4"/>
         <v>515</v>
@@ -3077,7 +3077,7 @@
         <f t="shared" si="9"/>
         <v>2.99</v>
       </c>
-      <c r="AA25" s="57"/>
+      <c r="AA25" s="62"/>
       <c r="AD25">
         <f t="shared" si="4"/>
         <v>412</v>
@@ -3160,7 +3160,7 @@
       <c r="Z26" s="26">
         <v>30</v>
       </c>
-      <c r="AA26" s="57"/>
+      <c r="AA26" s="62"/>
       <c r="AD26">
         <f t="shared" si="4"/>
         <v>330</v>
@@ -3267,7 +3267,7 @@
         <f t="shared" si="10"/>
         <v>2.093</v>
       </c>
-      <c r="AA27" s="57"/>
+      <c r="AA27" s="62"/>
       <c r="AD27">
         <f t="shared" si="4"/>
         <v>264</v>
@@ -3498,30 +3498,30 @@
       <c r="B30" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="61"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="61"/>
-      <c r="P30" s="61"/>
-      <c r="Q30" s="61"/>
-      <c r="R30" s="61"/>
-      <c r="S30" s="61"/>
-      <c r="T30" s="61"/>
-      <c r="U30" s="61"/>
-      <c r="V30" s="61"/>
-      <c r="W30" s="61"/>
-      <c r="X30" s="61"/>
-      <c r="Y30" s="61"/>
-      <c r="Z30" s="61"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="66"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
+      <c r="U30" s="66"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="66"/>
+      <c r="X30" s="66"/>
+      <c r="Y30" s="66"/>
+      <c r="Z30" s="66"/>
       <c r="AA30" s="34"/>
       <c r="AD30">
         <f t="shared" si="4"/>
@@ -3605,7 +3605,7 @@
       <c r="Z31" s="25">
         <v>19.989999999999998</v>
       </c>
-      <c r="AA31" s="56"/>
+      <c r="AA31" s="61"/>
       <c r="AD31">
         <f t="shared" si="4"/>
         <v>108</v>
@@ -3688,7 +3688,7 @@
       <c r="Z32" s="12">
         <v>10</v>
       </c>
-      <c r="AA32" s="57"/>
+      <c r="AA32" s="62"/>
       <c r="AD32">
         <f t="shared" si="4"/>
         <v>86</v>
@@ -3795,7 +3795,7 @@
         <f t="shared" si="13"/>
         <v>17.991</v>
       </c>
-      <c r="AA33" s="57"/>
+      <c r="AA33" s="62"/>
       <c r="AD33">
         <f t="shared" si="4"/>
         <v>69</v>
@@ -3807,78 +3807,78 @@
         <v>5</v>
       </c>
       <c r="C34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="T34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Y34" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Z34" s="26">
-        <v>30</v>
-      </c>
-      <c r="AA34" s="57"/>
+        <v>35</v>
+      </c>
+      <c r="AA34" s="62"/>
       <c r="AD34">
         <f t="shared" si="4"/>
         <v>55</v>
@@ -3891,101 +3891,101 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ref="C35:Z35" si="14">C33-(C33*C34/100)</f>
-        <v>11.194399999999998</v>
+        <v>10.3948</v>
       </c>
       <c r="D35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="E35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="F35" s="28">
         <f t="shared" si="14"/>
-        <v>11.194399999999998</v>
+        <v>10.3948</v>
       </c>
       <c r="G35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="H35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="I35" s="28">
         <f t="shared" si="14"/>
-        <v>11.194399999999998</v>
+        <v>10.3948</v>
       </c>
       <c r="J35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="K35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="L35" s="28">
         <f t="shared" si="14"/>
-        <v>11.194399999999998</v>
+        <v>10.3948</v>
       </c>
       <c r="M35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="O35" s="28">
         <f t="shared" si="14"/>
-        <v>9.0954499999999978</v>
+        <v>8.4457749999999976</v>
       </c>
       <c r="P35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="Q35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="R35" s="28">
         <f t="shared" si="14"/>
-        <v>9.0954499999999978</v>
+        <v>8.4457749999999976</v>
       </c>
       <c r="S35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="T35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="U35" s="28">
         <f t="shared" si="14"/>
-        <v>9.0954499999999978</v>
+        <v>8.4457749999999976</v>
       </c>
       <c r="V35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="W35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="X35" s="28">
         <f t="shared" si="14"/>
-        <v>9.0954499999999978</v>
+        <v>8.4457749999999976</v>
       </c>
       <c r="Y35" s="28">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
+        <v>11.69415</v>
       </c>
       <c r="Z35" s="13">
         <f t="shared" si="14"/>
-        <v>12.593699999999998</v>
-      </c>
-      <c r="AA35" s="57"/>
+        <v>11.69415</v>
+      </c>
+      <c r="AA35" s="62"/>
       <c r="AD35">
         <f t="shared" si="4"/>
         <v>44</v>
@@ -3996,109 +3996,100 @@
       <c r="B36" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="30">
         <f>AD13</f>
         <v>6000</v>
       </c>
-      <c r="D36" s="30">
+      <c r="G36" s="30">
         <f>AD14</f>
         <v>4800</v>
       </c>
-      <c r="E36" s="14">
+      <c r="H36" s="14">
         <f>AD15</f>
         <v>3840</v>
       </c>
-      <c r="F36" s="30">
+      <c r="I36" s="30">
         <f>AD16</f>
         <v>3072</v>
       </c>
-      <c r="G36" s="30">
+      <c r="J36" s="30">
         <f>AD17</f>
         <v>2458</v>
       </c>
-      <c r="H36" s="14">
+      <c r="K36" s="14">
         <f>AD18</f>
         <v>1966</v>
       </c>
-      <c r="I36" s="30">
+      <c r="L36" s="30">
         <f>AD19</f>
         <v>1573</v>
       </c>
-      <c r="J36" s="30">
+      <c r="M36" s="30">
         <f>AD20</f>
         <v>1258</v>
       </c>
-      <c r="K36" s="14">
+      <c r="N36" s="14">
         <f>AD21</f>
         <v>1006</v>
       </c>
-      <c r="L36" s="30">
+      <c r="O36" s="30">
         <f>AD22</f>
         <v>805</v>
       </c>
-      <c r="M36" s="30">
+      <c r="P36" s="30">
         <f>AD23</f>
         <v>644</v>
       </c>
-      <c r="N36" s="14">
+      <c r="Q36" s="14">
         <f>AD24</f>
         <v>515</v>
       </c>
-      <c r="O36" s="30">
+      <c r="R36" s="30">
         <f>AD25</f>
         <v>412</v>
       </c>
-      <c r="P36" s="30">
+      <c r="S36" s="30">
         <f>AD26</f>
         <v>330</v>
       </c>
-      <c r="Q36" s="14">
+      <c r="T36" s="14">
         <f>AD27</f>
         <v>264</v>
       </c>
-      <c r="R36" s="30">
+      <c r="U36" s="30">
         <f>AD28</f>
         <v>211</v>
       </c>
-      <c r="S36" s="30">
+      <c r="V36" s="30">
         <f>AD29</f>
         <v>169</v>
       </c>
-      <c r="T36" s="14">
+      <c r="W36" s="14">
         <f>AD30</f>
         <v>135</v>
       </c>
-      <c r="U36" s="30">
+      <c r="X36" s="30">
         <f>AD31</f>
         <v>108</v>
       </c>
-      <c r="V36" s="30">
+      <c r="Y36" s="30">
         <f>AD32</f>
         <v>86</v>
       </c>
-      <c r="W36" s="14">
+      <c r="Z36" s="14">
         <f>AD33</f>
         <v>69</v>
       </c>
-      <c r="X36" s="30">
-        <f>AD34</f>
-        <v>55</v>
-      </c>
-      <c r="Y36" s="30">
-        <f>AD35</f>
-        <v>44</v>
-      </c>
-      <c r="Z36" s="14">
-        <f>AD36</f>
-        <v>35</v>
-      </c>
       <c r="AA36" s="31">
         <f>SUM(C36:Z36)</f>
-        <v>29855</v>
+        <v>29721</v>
       </c>
       <c r="AB36" s="44">
         <f>SUM(C36:Z36)</f>
-        <v>29855</v>
+        <v>29721</v>
       </c>
       <c r="AD36">
         <f t="shared" si="4"/>
@@ -4122,108 +4113,108 @@
         <v>38</v>
       </c>
       <c r="C37" s="35">
-        <f t="shared" ref="C37:Z37" si="15">C35*C36</f>
-        <v>67166.399999999994</v>
+        <f>C35*C36</f>
+        <v>0</v>
       </c>
       <c r="D37" s="35">
-        <f t="shared" si="15"/>
-        <v>60449.759999999995</v>
+        <f>D35*D36</f>
+        <v>0</v>
       </c>
       <c r="E37" s="17">
-        <f t="shared" si="15"/>
-        <v>48359.80799999999</v>
+        <f>E35*E36</f>
+        <v>0</v>
       </c>
       <c r="F37" s="35">
-        <f t="shared" si="15"/>
-        <v>34389.196799999991</v>
+        <f>F35*F36</f>
+        <v>62368.800000000003</v>
       </c>
       <c r="G37" s="35">
-        <f t="shared" si="15"/>
-        <v>30955.314599999994</v>
+        <f>G35*G36</f>
+        <v>56131.920000000006</v>
       </c>
       <c r="H37" s="17">
-        <f t="shared" si="15"/>
-        <v>24759.214199999999</v>
+        <f>H35*H36</f>
+        <v>44905.536</v>
       </c>
       <c r="I37" s="35">
-        <f t="shared" si="15"/>
-        <v>17608.791199999996</v>
+        <f>I35*I36</f>
+        <v>31932.8256</v>
       </c>
       <c r="J37" s="35">
-        <f t="shared" si="15"/>
-        <v>15842.874599999997</v>
+        <f>J35*J36</f>
+        <v>28744.220700000002</v>
       </c>
       <c r="K37" s="17">
-        <f t="shared" si="15"/>
-        <v>12669.262199999999</v>
+        <f>K35*K36</f>
+        <v>22990.698899999999</v>
       </c>
       <c r="L37" s="35">
-        <f t="shared" si="15"/>
-        <v>9011.4919999999984</v>
+        <f>L35*L36</f>
+        <v>16351.020399999999</v>
       </c>
       <c r="M37" s="35">
-        <f t="shared" si="15"/>
-        <v>8110.3427999999985</v>
+        <f>M35*M36</f>
+        <v>14711.2407</v>
       </c>
       <c r="N37" s="17">
-        <f t="shared" si="15"/>
-        <v>6485.7554999999993</v>
+        <f>N35*N36</f>
+        <v>11764.314900000001</v>
       </c>
       <c r="O37" s="35">
-        <f t="shared" si="15"/>
-        <v>3747.3253999999993</v>
+        <f>O35*O36</f>
+        <v>6798.8488749999979</v>
       </c>
       <c r="P37" s="35">
-        <f t="shared" si="15"/>
-        <v>4155.9209999999994</v>
+        <f>P35*P36</f>
+        <v>7531.0326000000005</v>
       </c>
       <c r="Q37" s="17">
-        <f t="shared" si="15"/>
-        <v>3324.7367999999997</v>
+        <f>Q35*Q36</f>
+        <v>6022.4872500000001</v>
       </c>
       <c r="R37" s="35">
-        <f t="shared" si="15"/>
-        <v>1919.1399499999995</v>
+        <f>R35*R36</f>
+        <v>3479.6592999999989</v>
       </c>
       <c r="S37" s="35">
-        <f t="shared" si="15"/>
-        <v>2128.3352999999997</v>
+        <f>S35*S36</f>
+        <v>3859.0695000000001</v>
       </c>
       <c r="T37" s="17">
-        <f t="shared" si="15"/>
-        <v>1700.1494999999998</v>
+        <f>T35*T36</f>
+        <v>3087.2556</v>
       </c>
       <c r="U37" s="35">
-        <f t="shared" si="15"/>
-        <v>982.30859999999973</v>
+        <f>U35*U36</f>
+        <v>1782.0585249999995</v>
       </c>
       <c r="V37" s="35">
-        <f t="shared" si="15"/>
-        <v>1083.0581999999999</v>
+        <f>V35*V36</f>
+        <v>1976.3113500000002</v>
       </c>
       <c r="W37" s="17">
-        <f t="shared" si="15"/>
-        <v>868.96529999999984</v>
+        <f>W35*W36</f>
+        <v>1578.7102500000001</v>
       </c>
       <c r="X37" s="35">
-        <f t="shared" si="15"/>
-        <v>500.24974999999989</v>
+        <f>X35*X36</f>
+        <v>912.14369999999974</v>
       </c>
       <c r="Y37" s="35">
-        <f t="shared" si="15"/>
-        <v>554.12279999999987</v>
+        <f>Y35*Y36</f>
+        <v>1005.6969</v>
       </c>
       <c r="Z37" s="17">
-        <f t="shared" si="15"/>
-        <v>440.77949999999993</v>
+        <f>Z35*Z36</f>
+        <v>806.89634999999998</v>
       </c>
       <c r="AA37" s="36">
         <f>SUM(C37:Z37)</f>
-        <v>357213.30399999983</v>
+        <v>328740.74739999993</v>
       </c>
       <c r="AB37" s="9">
         <f>AB36*3</f>
-        <v>89565</v>
+        <v>89163</v>
       </c>
       <c r="AD37">
         <f t="shared" si="4"/>
@@ -4246,30 +4237,30 @@
       <c r="B38" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="60"/>
-      <c r="O38" s="60"/>
-      <c r="P38" s="60"/>
-      <c r="Q38" s="60"/>
-      <c r="R38" s="60"/>
-      <c r="S38" s="60"/>
-      <c r="T38" s="60"/>
-      <c r="U38" s="60"/>
-      <c r="V38" s="60"/>
-      <c r="W38" s="60"/>
-      <c r="X38" s="60"/>
-      <c r="Y38" s="60"/>
-      <c r="Z38" s="60"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="65"/>
+      <c r="O38" s="65"/>
+      <c r="P38" s="65"/>
+      <c r="Q38" s="65"/>
+      <c r="R38" s="65"/>
+      <c r="S38" s="65"/>
+      <c r="T38" s="65"/>
+      <c r="U38" s="65"/>
+      <c r="V38" s="65"/>
+      <c r="W38" s="65"/>
+      <c r="X38" s="65"/>
+      <c r="Y38" s="65"/>
+      <c r="Z38" s="65"/>
       <c r="AA38" s="34"/>
       <c r="AQ38" s="6"/>
       <c r="AR38" s="6"/>
@@ -4360,7 +4351,7 @@
       <c r="Z39" s="25">
         <v>19.989999999999998</v>
       </c>
-      <c r="AA39" s="62"/>
+      <c r="AA39" s="67"/>
       <c r="AQ39" s="6"/>
       <c r="AR39" s="6"/>
       <c r="AS39" s="6"/>
@@ -4450,7 +4441,7 @@
       <c r="Z40" s="12">
         <v>10</v>
       </c>
-      <c r="AA40" s="62"/>
+      <c r="AA40" s="67"/>
       <c r="AQ40" s="6"/>
       <c r="AR40" s="6"/>
       <c r="AS40" s="6"/>
@@ -4469,102 +4460,102 @@
         <v>4</v>
       </c>
       <c r="C41" s="28">
-        <f t="shared" ref="C41:Z41" si="16">C39-(C39*C40/100)</f>
+        <f t="shared" ref="C41:Z41" si="15">C39-(C39*C40/100)</f>
         <v>15.991999999999999</v>
       </c>
       <c r="D41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="E41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="F41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>15.991999999999999</v>
       </c>
       <c r="G41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="H41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="I41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>15.991999999999999</v>
       </c>
       <c r="J41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="K41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="L41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>15.991999999999999</v>
       </c>
       <c r="M41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="N41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="O41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>12.993499999999997</v>
       </c>
       <c r="P41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="Q41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="R41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>12.993499999999997</v>
       </c>
       <c r="S41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="T41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="U41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>12.993499999999997</v>
       </c>
       <c r="V41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="W41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="X41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>12.993499999999997</v>
       </c>
       <c r="Y41" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
       <c r="Z41" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>17.991</v>
       </c>
-      <c r="AA41" s="62"/>
+      <c r="AA41" s="67"/>
       <c r="AQ41" s="6"/>
       <c r="AR41" s="6"/>
       <c r="AS41" s="6"/>
@@ -4583,81 +4574,81 @@
         <v>5</v>
       </c>
       <c r="C42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="T42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Y42" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Z42" s="26">
-        <v>30</v>
-      </c>
-      <c r="AA42" s="62"/>
+        <v>35</v>
+      </c>
+      <c r="AA42" s="67"/>
       <c r="AB42" s="45">
         <f>AA37+AA45+AA53</f>
-        <v>1018031.1119999995</v>
+        <v>936886.46219999995</v>
       </c>
       <c r="AQ42" s="6"/>
       <c r="AR42" s="6"/>
@@ -4677,102 +4668,102 @@
         <v>6</v>
       </c>
       <c r="C43" s="28">
-        <f t="shared" ref="C43:Z43" si="17">C41-(C41*C42/100)</f>
-        <v>11.194399999999998</v>
+        <f t="shared" ref="C43:Z43" si="16">C41-(C41*C42/100)</f>
+        <v>10.3948</v>
       </c>
       <c r="D43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="E43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="F43" s="28">
-        <f t="shared" si="17"/>
-        <v>11.194399999999998</v>
+        <f t="shared" si="16"/>
+        <v>10.3948</v>
       </c>
       <c r="G43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="H43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="I43" s="28">
-        <f t="shared" si="17"/>
-        <v>11.194399999999998</v>
+        <f t="shared" si="16"/>
+        <v>10.3948</v>
       </c>
       <c r="J43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="K43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="L43" s="28">
-        <f t="shared" si="17"/>
-        <v>11.194399999999998</v>
+        <f t="shared" si="16"/>
+        <v>10.3948</v>
       </c>
       <c r="M43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="N43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="O43" s="28">
-        <f t="shared" si="17"/>
-        <v>9.0954499999999978</v>
+        <f t="shared" si="16"/>
+        <v>8.4457749999999976</v>
       </c>
       <c r="P43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="Q43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="R43" s="28">
-        <f t="shared" si="17"/>
-        <v>9.0954499999999978</v>
+        <f t="shared" si="16"/>
+        <v>8.4457749999999976</v>
       </c>
       <c r="S43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="T43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="U43" s="28">
-        <f t="shared" si="17"/>
-        <v>9.0954499999999978</v>
+        <f t="shared" si="16"/>
+        <v>8.4457749999999976</v>
       </c>
       <c r="V43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="W43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="X43" s="28">
-        <f t="shared" si="17"/>
-        <v>9.0954499999999978</v>
+        <f t="shared" si="16"/>
+        <v>8.4457749999999976</v>
       </c>
       <c r="Y43" s="28">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
       </c>
       <c r="Z43" s="13">
-        <f t="shared" si="17"/>
-        <v>12.593699999999998</v>
-      </c>
-      <c r="AA43" s="62"/>
+        <f t="shared" si="16"/>
+        <v>11.69415</v>
+      </c>
+      <c r="AA43" s="67"/>
       <c r="AQ43" s="6"/>
       <c r="AR43" s="6"/>
       <c r="AS43" s="6"/>
@@ -4790,105 +4781,75 @@
       <c r="B44" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="30">
-        <f>AD13</f>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="30">
         <v>6000</v>
       </c>
-      <c r="D44" s="30">
-        <f>AD14</f>
+      <c r="G44" s="30">
         <v>4800</v>
       </c>
-      <c r="E44" s="14">
-        <f>AD15</f>
+      <c r="H44" s="14">
         <v>3840</v>
       </c>
-      <c r="F44" s="30">
-        <f>AD16</f>
+      <c r="I44" s="30">
         <v>3072</v>
       </c>
-      <c r="G44" s="30">
-        <f>AD17</f>
+      <c r="J44" s="30">
         <v>2458</v>
       </c>
-      <c r="H44" s="14">
-        <f>AD18</f>
+      <c r="K44" s="14">
         <v>1966</v>
       </c>
-      <c r="I44" s="30">
-        <f>AD19</f>
+      <c r="L44" s="30">
         <v>1573</v>
       </c>
-      <c r="J44" s="30">
-        <f>AD20</f>
+      <c r="M44" s="30">
         <v>1258</v>
       </c>
-      <c r="K44" s="14">
-        <f>AD21</f>
+      <c r="N44" s="14">
         <v>1006</v>
       </c>
-      <c r="L44" s="30">
-        <f>AD22</f>
+      <c r="O44" s="30">
         <v>805</v>
       </c>
-      <c r="M44" s="30">
-        <f>AD23</f>
+      <c r="P44" s="30">
         <v>644</v>
       </c>
-      <c r="N44" s="14">
-        <f>AD24</f>
+      <c r="Q44" s="14">
         <v>515</v>
       </c>
-      <c r="O44" s="30">
-        <f>AD25</f>
+      <c r="R44" s="30">
         <v>412</v>
       </c>
-      <c r="P44" s="30">
-        <f>AD26</f>
+      <c r="S44" s="30">
         <v>330</v>
       </c>
-      <c r="Q44" s="14">
-        <f>AD27</f>
+      <c r="T44" s="14">
         <v>264</v>
       </c>
-      <c r="R44" s="30">
-        <f>AD28</f>
+      <c r="U44" s="30">
         <v>211</v>
       </c>
-      <c r="S44" s="30">
-        <f>AD29</f>
+      <c r="V44" s="30">
         <v>169</v>
       </c>
-      <c r="T44" s="14">
-        <f>AD30</f>
+      <c r="W44" s="14">
         <v>135</v>
       </c>
-      <c r="U44" s="30">
-        <f>AD31</f>
+      <c r="X44" s="30">
         <v>108</v>
       </c>
-      <c r="V44" s="30">
-        <f>AD32</f>
+      <c r="Y44" s="30">
         <v>86</v>
       </c>
-      <c r="W44" s="14">
-        <f>AD33</f>
+      <c r="Z44" s="14">
         <v>69</v>
-      </c>
-      <c r="X44" s="30">
-        <f>AD34</f>
-        <v>55</v>
-      </c>
-      <c r="Y44" s="30">
-        <f>AD35</f>
-        <v>44</v>
-      </c>
-      <c r="Z44" s="14">
-        <f>AD36</f>
-        <v>35</v>
       </c>
       <c r="AA44" s="31">
         <f>SUM(C44:Z44)</f>
-        <v>29855</v>
+        <v>29721</v>
       </c>
       <c r="AQ44" s="6"/>
       <c r="AR44" s="6"/>
@@ -4908,104 +4869,104 @@
         <v>39</v>
       </c>
       <c r="C45" s="35">
-        <f t="shared" ref="C45:Z45" si="18">C43*C44</f>
-        <v>67166.399999999994</v>
+        <f t="shared" ref="C45:Z45" si="17">C43*C44</f>
+        <v>0</v>
       </c>
       <c r="D45" s="35">
-        <f t="shared" si="18"/>
-        <v>60449.759999999995</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="E45" s="17">
-        <f t="shared" si="18"/>
-        <v>48359.80799999999</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="F45" s="35">
-        <f t="shared" si="18"/>
-        <v>34389.196799999991</v>
+        <f t="shared" si="17"/>
+        <v>62368.800000000003</v>
       </c>
       <c r="G45" s="35">
-        <f t="shared" si="18"/>
-        <v>30955.314599999994</v>
+        <f t="shared" si="17"/>
+        <v>56131.920000000006</v>
       </c>
       <c r="H45" s="17">
-        <f t="shared" si="18"/>
-        <v>24759.214199999999</v>
+        <f t="shared" si="17"/>
+        <v>44905.536</v>
       </c>
       <c r="I45" s="35">
-        <f t="shared" si="18"/>
-        <v>17608.791199999996</v>
+        <f t="shared" si="17"/>
+        <v>31932.8256</v>
       </c>
       <c r="J45" s="35">
-        <f t="shared" si="18"/>
-        <v>15842.874599999997</v>
+        <f t="shared" si="17"/>
+        <v>28744.220700000002</v>
       </c>
       <c r="K45" s="17">
-        <f t="shared" si="18"/>
-        <v>12669.262199999999</v>
+        <f t="shared" si="17"/>
+        <v>22990.698899999999</v>
       </c>
       <c r="L45" s="35">
-        <f t="shared" si="18"/>
-        <v>9011.4919999999984</v>
+        <f t="shared" si="17"/>
+        <v>16351.020399999999</v>
       </c>
       <c r="M45" s="35">
-        <f t="shared" si="18"/>
-        <v>8110.3427999999985</v>
+        <f t="shared" si="17"/>
+        <v>14711.2407</v>
       </c>
       <c r="N45" s="17">
-        <f t="shared" si="18"/>
-        <v>6485.7554999999993</v>
+        <f t="shared" si="17"/>
+        <v>11764.314900000001</v>
       </c>
       <c r="O45" s="35">
-        <f t="shared" si="18"/>
-        <v>3747.3253999999993</v>
+        <f t="shared" si="17"/>
+        <v>6798.8488749999979</v>
       </c>
       <c r="P45" s="35">
-        <f t="shared" si="18"/>
-        <v>4155.9209999999994</v>
+        <f t="shared" si="17"/>
+        <v>7531.0326000000005</v>
       </c>
       <c r="Q45" s="17">
-        <f t="shared" si="18"/>
-        <v>3324.7367999999997</v>
+        <f t="shared" si="17"/>
+        <v>6022.4872500000001</v>
       </c>
       <c r="R45" s="35">
-        <f t="shared" si="18"/>
-        <v>1919.1399499999995</v>
+        <f t="shared" si="17"/>
+        <v>3479.6592999999989</v>
       </c>
       <c r="S45" s="35">
-        <f t="shared" si="18"/>
-        <v>2128.3352999999997</v>
+        <f t="shared" si="17"/>
+        <v>3859.0695000000001</v>
       </c>
       <c r="T45" s="17">
-        <f t="shared" si="18"/>
-        <v>1700.1494999999998</v>
+        <f t="shared" si="17"/>
+        <v>3087.2556</v>
       </c>
       <c r="U45" s="35">
-        <f t="shared" si="18"/>
-        <v>982.30859999999973</v>
+        <f t="shared" si="17"/>
+        <v>1782.0585249999995</v>
       </c>
       <c r="V45" s="35">
-        <f t="shared" si="18"/>
-        <v>1083.0581999999999</v>
+        <f t="shared" si="17"/>
+        <v>1976.3113500000002</v>
       </c>
       <c r="W45" s="17">
-        <f t="shared" si="18"/>
-        <v>868.96529999999984</v>
+        <f t="shared" si="17"/>
+        <v>1578.7102500000001</v>
       </c>
       <c r="X45" s="35">
-        <f t="shared" si="18"/>
-        <v>500.24974999999989</v>
+        <f t="shared" si="17"/>
+        <v>912.14369999999974</v>
       </c>
       <c r="Y45" s="35">
-        <f t="shared" si="18"/>
-        <v>554.12279999999987</v>
+        <f t="shared" si="17"/>
+        <v>1005.6969</v>
       </c>
       <c r="Z45" s="17">
-        <f t="shared" si="18"/>
-        <v>440.77949999999993</v>
+        <f t="shared" si="17"/>
+        <v>806.89634999999998</v>
       </c>
       <c r="AA45" s="36">
         <f>SUM(C45:Z45)</f>
-        <v>357213.30399999983</v>
+        <v>328740.74739999993</v>
       </c>
       <c r="AQ45" s="6"/>
       <c r="AR45" s="6"/>
@@ -5024,30 +4985,30 @@
       <c r="B46" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="60"/>
-      <c r="I46" s="60"/>
-      <c r="J46" s="60"/>
-      <c r="K46" s="60"/>
-      <c r="L46" s="60"/>
-      <c r="M46" s="60"/>
-      <c r="N46" s="60"/>
-      <c r="O46" s="60"/>
-      <c r="P46" s="60"/>
-      <c r="Q46" s="60"/>
-      <c r="R46" s="60"/>
-      <c r="S46" s="60"/>
-      <c r="T46" s="60"/>
-      <c r="U46" s="60"/>
-      <c r="V46" s="60"/>
-      <c r="W46" s="60"/>
-      <c r="X46" s="60"/>
-      <c r="Y46" s="60"/>
-      <c r="Z46" s="60"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="65"/>
+      <c r="J46" s="65"/>
+      <c r="K46" s="65"/>
+      <c r="L46" s="65"/>
+      <c r="M46" s="65"/>
+      <c r="N46" s="65"/>
+      <c r="O46" s="65"/>
+      <c r="P46" s="65"/>
+      <c r="Q46" s="65"/>
+      <c r="R46" s="65"/>
+      <c r="S46" s="65"/>
+      <c r="T46" s="65"/>
+      <c r="U46" s="65"/>
+      <c r="V46" s="65"/>
+      <c r="W46" s="65"/>
+      <c r="X46" s="65"/>
+      <c r="Y46" s="65"/>
+      <c r="Z46" s="65"/>
       <c r="AA46" s="34"/>
     </row>
     <row r="47" spans="1:53" ht="15" x14ac:dyDescent="0.3">
@@ -5127,7 +5088,7 @@
       <c r="Z47" s="25">
         <v>16.989999999999998</v>
       </c>
-      <c r="AA47" s="62"/>
+      <c r="AA47" s="67"/>
     </row>
     <row r="48" spans="1:53" ht="15" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
@@ -5206,7 +5167,7 @@
       <c r="Z48" s="12">
         <v>10</v>
       </c>
-      <c r="AA48" s="62"/>
+      <c r="AA48" s="67"/>
     </row>
     <row r="49" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
@@ -5214,102 +5175,102 @@
         <v>4</v>
       </c>
       <c r="C49" s="28">
-        <f t="shared" ref="C49:Z49" si="19">C47-(C47*C48/100)</f>
+        <f t="shared" ref="C49:Z49" si="18">C47-(C47*C48/100)</f>
         <v>13.591999999999999</v>
       </c>
       <c r="D49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="E49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="F49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>13.591999999999999</v>
       </c>
       <c r="G49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="H49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="I49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>13.591999999999999</v>
       </c>
       <c r="J49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="K49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="L49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>13.591999999999999</v>
       </c>
       <c r="M49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="N49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="O49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>11.043499999999998</v>
       </c>
       <c r="P49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="Q49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="R49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>11.043499999999998</v>
       </c>
       <c r="S49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="T49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="U49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>11.043499999999998</v>
       </c>
       <c r="V49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="W49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="X49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>11.043499999999998</v>
       </c>
       <c r="Y49" s="28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
       <c r="Z49" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>15.290999999999999</v>
       </c>
-      <c r="AA49" s="62"/>
+      <c r="AA49" s="67"/>
     </row>
     <row r="50" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
@@ -5317,78 +5278,78 @@
         <v>5</v>
       </c>
       <c r="C50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="T50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Y50" s="26">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Z50" s="26">
-        <v>30</v>
-      </c>
-      <c r="AA50" s="62"/>
+        <v>35</v>
+      </c>
+      <c r="AA50" s="67"/>
     </row>
     <row r="51" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
@@ -5396,207 +5357,177 @@
         <v>6</v>
       </c>
       <c r="C51" s="28">
-        <f t="shared" ref="C51:Z51" si="20">C49-(C49*C50/100)</f>
-        <v>9.5143999999999984</v>
+        <f t="shared" ref="C51:Z51" si="19">C49-(C49*C50/100)</f>
+        <v>8.8347999999999978</v>
       </c>
       <c r="D51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="E51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="F51" s="28">
-        <f t="shared" si="20"/>
-        <v>9.5143999999999984</v>
+        <f t="shared" si="19"/>
+        <v>8.8347999999999978</v>
       </c>
       <c r="G51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="H51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="I51" s="28">
-        <f t="shared" si="20"/>
-        <v>9.5143999999999984</v>
+        <f t="shared" si="19"/>
+        <v>8.8347999999999978</v>
       </c>
       <c r="J51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="K51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="L51" s="28">
-        <f t="shared" si="20"/>
-        <v>9.5143999999999984</v>
+        <f t="shared" si="19"/>
+        <v>8.8347999999999978</v>
       </c>
       <c r="M51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="N51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="O51" s="28">
-        <f t="shared" si="20"/>
-        <v>7.7304499999999985</v>
+        <f t="shared" si="19"/>
+        <v>7.1782749999999993</v>
       </c>
       <c r="P51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="Q51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="R51" s="28">
-        <f t="shared" si="20"/>
-        <v>7.7304499999999985</v>
+        <f t="shared" si="19"/>
+        <v>7.1782749999999993</v>
       </c>
       <c r="S51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="T51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="U51" s="28">
-        <f t="shared" si="20"/>
-        <v>7.7304499999999985</v>
+        <f t="shared" si="19"/>
+        <v>7.1782749999999993</v>
       </c>
       <c r="V51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="W51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="X51" s="28">
-        <f t="shared" si="20"/>
-        <v>7.7304499999999985</v>
+        <f t="shared" si="19"/>
+        <v>7.1782749999999993</v>
       </c>
       <c r="Y51" s="28">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
       </c>
       <c r="Z51" s="13">
-        <f t="shared" si="20"/>
-        <v>10.703699999999998</v>
-      </c>
-      <c r="AA51" s="62"/>
+        <f t="shared" si="19"/>
+        <v>9.9391499999999979</v>
+      </c>
+      <c r="AA51" s="67"/>
     </row>
     <row r="52" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="30">
-        <f>AD13</f>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="30">
         <v>6000</v>
       </c>
-      <c r="D52" s="30">
-        <f>AD14</f>
+      <c r="G52" s="30">
         <v>4800</v>
       </c>
-      <c r="E52" s="14">
-        <f>AD15</f>
+      <c r="H52" s="14">
         <v>3840</v>
       </c>
-      <c r="F52" s="30">
-        <f>AD16</f>
+      <c r="I52" s="30">
         <v>3072</v>
       </c>
-      <c r="G52" s="30">
-        <f>AD17</f>
+      <c r="J52" s="30">
         <v>2458</v>
       </c>
-      <c r="H52" s="14">
-        <f>AD18</f>
+      <c r="K52" s="14">
         <v>1966</v>
       </c>
-      <c r="I52" s="30">
-        <f>AD19</f>
+      <c r="L52" s="30">
         <v>1573</v>
       </c>
-      <c r="J52" s="30">
-        <f>AD20</f>
+      <c r="M52" s="30">
         <v>1258</v>
       </c>
-      <c r="K52" s="14">
-        <f>AD21</f>
+      <c r="N52" s="14">
         <v>1006</v>
       </c>
-      <c r="L52" s="30">
-        <f>AD22</f>
+      <c r="O52" s="30">
         <v>805</v>
       </c>
-      <c r="M52" s="30">
-        <f>AD23</f>
+      <c r="P52" s="30">
         <v>644</v>
       </c>
-      <c r="N52" s="14">
-        <f>AD24</f>
+      <c r="Q52" s="14">
         <v>515</v>
       </c>
-      <c r="O52" s="30">
-        <f>AD25</f>
+      <c r="R52" s="30">
         <v>412</v>
       </c>
-      <c r="P52" s="30">
-        <f>AD26</f>
+      <c r="S52" s="30">
         <v>330</v>
       </c>
-      <c r="Q52" s="14">
-        <f>AD27</f>
+      <c r="T52" s="14">
         <v>264</v>
       </c>
-      <c r="R52" s="30">
-        <f>AD28</f>
+      <c r="U52" s="30">
         <v>211</v>
       </c>
-      <c r="S52" s="30">
-        <f>AD29</f>
+      <c r="V52" s="30">
         <v>169</v>
       </c>
-      <c r="T52" s="14">
-        <f>AD30</f>
+      <c r="W52" s="14">
         <v>135</v>
       </c>
-      <c r="U52" s="30">
-        <f>AD31</f>
+      <c r="X52" s="30">
         <v>108</v>
       </c>
-      <c r="V52" s="30">
-        <f>AD32</f>
+      <c r="Y52" s="30">
         <v>86</v>
       </c>
-      <c r="W52" s="14">
-        <f>AD33</f>
+      <c r="Z52" s="14">
         <v>69</v>
-      </c>
-      <c r="X52" s="30">
-        <f>AD34</f>
-        <v>55</v>
-      </c>
-      <c r="Y52" s="30">
-        <f>AD35</f>
-        <v>44</v>
-      </c>
-      <c r="Z52" s="14">
-        <f>AD36</f>
-        <v>35</v>
       </c>
       <c r="AA52" s="31">
         <f>SUM(C52:Z52)</f>
-        <v>29855</v>
+        <v>29721</v>
       </c>
     </row>
     <row r="53" spans="1:27" thickBot="1" x14ac:dyDescent="0.35">
@@ -5605,104 +5536,104 @@
         <v>40</v>
       </c>
       <c r="C53" s="35">
-        <f t="shared" ref="C53:Z53" si="21">C51*C52</f>
-        <v>57086.399999999987</v>
+        <f t="shared" ref="C53:Z53" si="20">C51*C52</f>
+        <v>0</v>
       </c>
       <c r="D53" s="35">
-        <f t="shared" si="21"/>
-        <v>51377.759999999987</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="E53" s="17">
-        <f t="shared" si="21"/>
-        <v>41102.207999999991</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="F53" s="35">
-        <f t="shared" si="21"/>
-        <v>29228.236799999995</v>
+        <f t="shared" si="20"/>
+        <v>53008.799999999988</v>
       </c>
       <c r="G53" s="35">
-        <f t="shared" si="21"/>
-        <v>26309.694599999995</v>
+        <f t="shared" si="20"/>
+        <v>47707.919999999991</v>
       </c>
       <c r="H53" s="17">
-        <f t="shared" si="21"/>
-        <v>21043.474199999997</v>
+        <f t="shared" si="20"/>
+        <v>38166.335999999996</v>
       </c>
       <c r="I53" s="35">
-        <f t="shared" si="21"/>
-        <v>14966.151199999997</v>
+        <f t="shared" si="20"/>
+        <v>27140.505599999993</v>
       </c>
       <c r="J53" s="35">
-        <f t="shared" si="21"/>
-        <v>13465.254599999997</v>
+        <f t="shared" si="20"/>
+        <v>24430.430699999994</v>
       </c>
       <c r="K53" s="17">
-        <f t="shared" si="21"/>
-        <v>10767.922199999997</v>
+        <f t="shared" si="20"/>
+        <v>19540.368899999998</v>
       </c>
       <c r="L53" s="35">
-        <f t="shared" si="21"/>
-        <v>7659.0919999999987</v>
+        <f t="shared" si="20"/>
+        <v>13897.140399999997</v>
       </c>
       <c r="M53" s="35">
-        <f t="shared" si="21"/>
-        <v>6893.1827999999987</v>
+        <f t="shared" si="20"/>
+        <v>12503.450699999998</v>
       </c>
       <c r="N53" s="17">
-        <f t="shared" si="21"/>
-        <v>5512.4054999999989</v>
+        <f t="shared" si="20"/>
+        <v>9998.7848999999987</v>
       </c>
       <c r="O53" s="35">
-        <f t="shared" si="21"/>
-        <v>3184.9453999999992</v>
+        <f t="shared" si="20"/>
+        <v>5778.5113749999991</v>
       </c>
       <c r="P53" s="35">
-        <f t="shared" si="21"/>
-        <v>3532.2209999999991</v>
+        <f t="shared" si="20"/>
+        <v>6400.8125999999984</v>
       </c>
       <c r="Q53" s="17">
-        <f t="shared" si="21"/>
-        <v>2825.7767999999996</v>
+        <f t="shared" si="20"/>
+        <v>5118.6622499999985</v>
       </c>
       <c r="R53" s="35">
-        <f t="shared" si="21"/>
-        <v>1631.1249499999997</v>
+        <f t="shared" si="20"/>
+        <v>2957.4492999999998</v>
       </c>
       <c r="S53" s="35">
-        <f t="shared" si="21"/>
-        <v>1808.9252999999997</v>
+        <f t="shared" si="20"/>
+        <v>3279.9194999999995</v>
       </c>
       <c r="T53" s="17">
-        <f t="shared" si="21"/>
-        <v>1444.9994999999997</v>
+        <f t="shared" si="20"/>
+        <v>2623.9355999999993</v>
       </c>
       <c r="U53" s="35">
-        <f t="shared" si="21"/>
-        <v>834.88859999999988</v>
+        <f t="shared" si="20"/>
+        <v>1514.6160249999998</v>
       </c>
       <c r="V53" s="35">
-        <f t="shared" si="21"/>
-        <v>920.51819999999975</v>
+        <f t="shared" si="20"/>
+        <v>1679.7163499999997</v>
       </c>
       <c r="W53" s="17">
-        <f t="shared" si="21"/>
-        <v>738.55529999999987</v>
+        <f t="shared" si="20"/>
+        <v>1341.7852499999997</v>
       </c>
       <c r="X53" s="35">
-        <f t="shared" si="21"/>
-        <v>425.1747499999999</v>
+        <f t="shared" si="20"/>
+        <v>775.25369999999998</v>
       </c>
       <c r="Y53" s="35">
-        <f t="shared" si="21"/>
-        <v>470.9627999999999</v>
+        <f t="shared" si="20"/>
+        <v>854.76689999999985</v>
       </c>
       <c r="Z53" s="17">
-        <f t="shared" si="21"/>
-        <v>374.62949999999989</v>
+        <f t="shared" si="20"/>
+        <v>685.80134999999984</v>
       </c>
       <c r="AA53" s="36">
         <f>SUM(C53:Z53)</f>
-        <v>303604.5039999999</v>
+        <v>279404.96740000002</v>
       </c>
     </row>
     <row r="54" spans="1:27" thickTop="1" x14ac:dyDescent="0.3">
@@ -5712,103 +5643,103 @@
       </c>
       <c r="C54" s="5">
         <f>C28+C12+C36+C44+C52</f>
-        <v>51200</v>
+        <v>27200</v>
       </c>
       <c r="D54" s="5">
         <f>D28+D12+D36+D44+D52</f>
-        <v>20900</v>
+        <v>5600</v>
       </c>
       <c r="E54" s="5">
         <f>E28+E12+E36+E44+E52</f>
-        <v>14470</v>
+        <v>2680</v>
       </c>
       <c r="F54" s="5">
         <f>F28+F12+F36+F44+F52</f>
-        <v>11266</v>
+        <v>19920</v>
       </c>
       <c r="G54" s="5">
         <f>G28+G12+G36+G44+G52</f>
-        <v>14924</v>
+        <v>21880</v>
       </c>
       <c r="H54" s="5">
         <f>H28+H12+H36+H44+H52</f>
-        <v>8068</v>
+        <v>13660</v>
       </c>
       <c r="I54" s="5">
         <f>I28+I12+I36+I44+I52</f>
-        <v>6029</v>
+        <v>10526</v>
       </c>
       <c r="J54" s="5">
         <f>J28+J12+J36+J44+J52</f>
-        <v>4904</v>
+        <v>8504</v>
       </c>
       <c r="K54" s="5">
         <f>K28+K12+K36+K44+K52</f>
-        <v>10088</v>
+        <v>12968</v>
       </c>
       <c r="L54" s="5">
         <f>L28+L12+L36+L44+L52</f>
-        <v>4345</v>
+        <v>6649</v>
       </c>
       <c r="M54" s="5">
         <f>M28+M12+M36+M44+M52</f>
-        <v>3202</v>
+        <v>5044</v>
       </c>
       <c r="N54" s="5">
         <f>N28+N12+N36+N44+N52</f>
-        <v>2675</v>
+        <v>4148</v>
       </c>
       <c r="O54" s="5">
         <f>O28+O12+O36+O44+O52</f>
-        <v>8306</v>
+        <v>9485</v>
       </c>
       <c r="P54" s="5">
         <f>P28+P12+P36+P44+P52</f>
-        <v>2920</v>
+        <v>3862</v>
       </c>
       <c r="Q54" s="5">
         <f>Q28+Q12+Q36+Q44+Q52</f>
-        <v>2062</v>
+        <v>2815</v>
       </c>
       <c r="R54" s="5">
         <f>R28+R12+R36+R44+R52</f>
-        <v>1763</v>
+        <v>2366</v>
       </c>
       <c r="S54" s="5">
         <f>S28+S12+S36+S44+S52</f>
-        <v>7577</v>
+        <v>8060</v>
       </c>
       <c r="T54" s="5">
         <f>T28+T12+T36+T44+T52</f>
-        <v>2335</v>
+        <v>2722</v>
       </c>
       <c r="U54" s="5">
         <f>U28+U12+U36+U44+U52</f>
-        <v>1594</v>
+        <v>1903</v>
       </c>
       <c r="V54" s="5">
         <f>V28+V12+V36+V44+V52</f>
-        <v>1388</v>
+        <v>1637</v>
       </c>
       <c r="W54" s="5">
         <f>W28+W12+W36+W44+W52</f>
-        <v>7277</v>
+        <v>7475</v>
       </c>
       <c r="X54" s="5">
         <f>X28+X12+X36+X44+X52</f>
-        <v>2095</v>
+        <v>2254</v>
       </c>
       <c r="Y54" s="5">
         <f>Y28+Y12+Y36+Y44+Y52</f>
-        <v>1402</v>
+        <v>1528</v>
       </c>
       <c r="Z54" s="5">
         <f>Z28+Z12+Z36+Z44+Z52</f>
-        <v>1235</v>
+        <v>1337</v>
       </c>
       <c r="AA54" s="38">
         <f>SUM(C54:Z54)</f>
-        <v>192025</v>
+        <v>184223</v>
       </c>
     </row>
     <row r="55" spans="1:27" ht="15" x14ac:dyDescent="0.3">
@@ -5817,104 +5748,104 @@
         <v>11</v>
       </c>
       <c r="C55" s="46">
-        <f>C13+C21+C29+C37+C45+C53</f>
-        <v>323569.8</v>
+        <f t="shared" ref="C55:Z55" si="21">C13+C21+C29+C37+C45+C53</f>
+        <v>108660</v>
       </c>
       <c r="D55" s="46">
-        <f>D13+D21+D29+D37+D45+D53</f>
-        <v>204114.92999999996</v>
+        <f t="shared" si="21"/>
+        <v>27307.32</v>
       </c>
       <c r="E55" s="46">
-        <f>E13+E21+E29+E37+E45+E53</f>
-        <v>151966.11899999998</v>
+        <f t="shared" si="21"/>
+        <v>12785.196</v>
       </c>
       <c r="F55" s="46">
-        <f>F13+F21+F29+F37+F45+F53</f>
-        <v>106981.64539999998</v>
+        <f t="shared" si="21"/>
+        <v>186212.45199999999</v>
       </c>
       <c r="G55" s="46">
-        <f>G13+G21+G29+G37+G45+G53</f>
-        <v>125695.91879999998</v>
+        <f t="shared" si="21"/>
+        <v>197094.99599999998</v>
       </c>
       <c r="H55" s="46">
-        <f>H13+H21+H29+H37+H45+H53</f>
-        <v>80991.4476</v>
+        <f t="shared" si="21"/>
+        <v>138255.94199999998</v>
       </c>
       <c r="I55" s="46">
-        <f>I13+I21+I29+I37+I45+I53</f>
-        <v>56017.530599999984</v>
+        <f t="shared" si="21"/>
+        <v>96839.953799999988</v>
       </c>
       <c r="J55" s="46">
-        <f>J13+J21+J29+J37+J45+J53</f>
-        <v>50398.384799999985</v>
+        <f t="shared" si="21"/>
+        <v>87166.253100000002</v>
       </c>
       <c r="K55" s="46">
-        <f>K13+K21+K29+K37+K45+K53</f>
-        <v>71254.005599999989</v>
+        <f t="shared" si="21"/>
+        <v>100669.3257</v>
       </c>
       <c r="L55" s="46">
-        <f>L13+L21+L29+L37+L45+L53</f>
-        <v>33916.118999999992</v>
+        <f t="shared" si="21"/>
+        <v>54833.224199999997</v>
       </c>
       <c r="M55" s="46">
-        <f>M13+M21+M29+M37+M45+M53</f>
-        <v>29065.967399999998</v>
+        <f t="shared" si="21"/>
+        <v>47878.031099999993</v>
       </c>
       <c r="N55" s="46">
-        <f>N13+N21+N29+N37+N45+N53</f>
-        <v>23731.297500000001</v>
+        <f t="shared" si="21"/>
+        <v>38774.795700000002</v>
       </c>
       <c r="O55" s="46">
-        <f>O13+O21+O29+O37+O45+O53</f>
-        <v>32247.351199999997</v>
+        <f t="shared" si="21"/>
+        <v>40943.964124999999</v>
       </c>
       <c r="P55" s="46">
-        <f>P13+P21+P29+P37+P45+P53</f>
-        <v>21118.403999999995</v>
+        <f t="shared" si="21"/>
+        <v>30737.218799999995</v>
       </c>
       <c r="Q55" s="46">
-        <f>Q13+Q21+Q29+Q37+Q45+Q53</f>
-        <v>15427.349399999999</v>
+        <f t="shared" si="21"/>
+        <v>23115.735749999996</v>
       </c>
       <c r="R55" s="46">
-        <f>R13+R21+R29+R37+R45+R53</f>
-        <v>10425.949849999999</v>
+        <f t="shared" si="21"/>
+        <v>14873.312899999999</v>
       </c>
       <c r="S55" s="46">
-        <f>S13+S21+S29+S37+S45+S53</f>
-        <v>41213.154899999994</v>
+        <f t="shared" si="21"/>
+        <v>46145.617499999986</v>
       </c>
       <c r="T55" s="46">
-        <f>T13+T21+T29+T37+T45+T53</f>
-        <v>14119.639499999999</v>
+        <f t="shared" si="21"/>
+        <v>18072.787800000002</v>
       </c>
       <c r="U55" s="46">
-        <f>U13+U21+U29+U37+U45+U53</f>
-        <v>8147.5607999999993</v>
+        <f t="shared" si="21"/>
+        <v>10426.788074999999</v>
       </c>
       <c r="V55" s="46">
-        <f>V13+V21+V29+V37+V45+V53</f>
-        <v>8334.0155999999988</v>
+        <f t="shared" si="21"/>
+        <v>10879.72005</v>
       </c>
       <c r="W55" s="46">
-        <f>W13+W21+W29+W37+W45+W53</f>
-        <v>37624.044899999986</v>
+        <f t="shared" si="21"/>
+        <v>39646.764750000002</v>
       </c>
       <c r="X55" s="46">
-        <f>X13+X21+X29+X37+X45+X53</f>
-        <v>8619.419249999999</v>
+        <f t="shared" si="21"/>
+        <v>9793.2860999999994</v>
       </c>
       <c r="Y55" s="46">
-        <f>Y13+Y21+Y29+Y37+Y45+Y53</f>
-        <v>7531.3074000000006</v>
+        <f t="shared" si="21"/>
+        <v>8818.2597000000005</v>
       </c>
       <c r="Z55" s="46">
-        <f>Z13+Z21+Z29+Z37+Z45+Z53</f>
-        <v>6503.5694999999987</v>
+        <f t="shared" si="21"/>
+        <v>7546.9750499999991</v>
       </c>
       <c r="AA55" s="47">
         <f>SUM(C55:Z55)</f>
-        <v>1469014.932</v>
+        <v>1357477.9201999998</v>
       </c>
     </row>
     <row r="56" spans="1:27" thickBot="1" x14ac:dyDescent="0.35">
@@ -5924,99 +5855,99 @@
       </c>
       <c r="C56" s="48">
         <f>C55</f>
-        <v>323569.8</v>
+        <v>108660</v>
       </c>
       <c r="D56" s="48">
         <f t="shared" ref="D56:Z56" si="22">D55+C56</f>
-        <v>527684.73</v>
+        <v>135967.32</v>
       </c>
       <c r="E56" s="49">
         <f t="shared" si="22"/>
-        <v>679650.84899999993</v>
+        <v>148752.516</v>
       </c>
       <c r="F56" s="48">
         <f t="shared" si="22"/>
-        <v>786632.49439999997</v>
+        <v>334964.96799999999</v>
       </c>
       <c r="G56" s="48">
         <f t="shared" si="22"/>
-        <v>912328.41319999995</v>
+        <v>532059.96399999992</v>
       </c>
       <c r="H56" s="49">
         <f t="shared" si="22"/>
-        <v>993319.86079999991</v>
+        <v>670315.90599999996</v>
       </c>
       <c r="I56" s="48">
         <f t="shared" si="22"/>
-        <v>1049337.3913999998</v>
+        <v>767155.85979999998</v>
       </c>
       <c r="J56" s="48">
         <f t="shared" si="22"/>
-        <v>1099735.7761999997</v>
+        <v>854322.11289999995</v>
       </c>
       <c r="K56" s="49">
         <f t="shared" si="22"/>
-        <v>1170989.7817999998</v>
+        <v>954991.43859999999</v>
       </c>
       <c r="L56" s="48">
         <f t="shared" si="22"/>
-        <v>1204905.9007999997</v>
+        <v>1009824.6628</v>
       </c>
       <c r="M56" s="48">
         <f t="shared" si="22"/>
-        <v>1233971.8681999997</v>
+        <v>1057702.6939000001</v>
       </c>
       <c r="N56" s="49">
         <f t="shared" si="22"/>
-        <v>1257703.1656999998</v>
+        <v>1096477.4896</v>
       </c>
       <c r="O56" s="48">
         <f t="shared" si="22"/>
-        <v>1289950.5168999997</v>
+        <v>1137421.4537249999</v>
       </c>
       <c r="P56" s="48">
         <f t="shared" si="22"/>
-        <v>1311068.9208999998</v>
+        <v>1168158.6725249998</v>
       </c>
       <c r="Q56" s="49">
         <f t="shared" si="22"/>
-        <v>1326496.2702999997</v>
+        <v>1191274.4082749998</v>
       </c>
       <c r="R56" s="48">
         <f t="shared" si="22"/>
-        <v>1336922.2201499997</v>
+        <v>1206147.7211749998</v>
       </c>
       <c r="S56" s="48">
         <f t="shared" si="22"/>
-        <v>1378135.3750499997</v>
+        <v>1252293.3386749998</v>
       </c>
       <c r="T56" s="49">
         <f t="shared" si="22"/>
-        <v>1392255.0145499997</v>
+        <v>1270366.1264749998</v>
       </c>
       <c r="U56" s="48">
         <f t="shared" si="22"/>
-        <v>1400402.5753499998</v>
+        <v>1280792.9145499999</v>
       </c>
       <c r="V56" s="48">
         <f t="shared" si="22"/>
-        <v>1408736.5909499999</v>
+        <v>1291672.6345999998</v>
       </c>
       <c r="W56" s="49">
         <f t="shared" si="22"/>
-        <v>1446360.63585</v>
+        <v>1331319.3993499998</v>
       </c>
       <c r="X56" s="48">
         <f t="shared" si="22"/>
-        <v>1454980.0551</v>
+        <v>1341112.6854499998</v>
       </c>
       <c r="Y56" s="48">
         <f t="shared" si="22"/>
-        <v>1462511.3625</v>
+        <v>1349930.9451499998</v>
       </c>
       <c r="Z56" s="49">
         <f t="shared" si="22"/>
-        <v>1469014.932</v>
+        <v>1357477.9201999998</v>
       </c>
       <c r="AA56" s="50"/>
     </row>
@@ -6056,21 +5987,21 @@
       <c r="C58" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="51" t="s">
+      <c r="D58" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="52"/>
-      <c r="K58" s="52"/>
-      <c r="L58" s="52"/>
-      <c r="M58" s="52"/>
-      <c r="N58" s="52"/>
-      <c r="O58" s="52"/>
-      <c r="P58" s="52"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
+      <c r="L58" s="57"/>
+      <c r="M58" s="57"/>
+      <c r="N58" s="57"/>
+      <c r="O58" s="57"/>
+      <c r="P58" s="57"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
@@ -6091,21 +6022,21 @@
       <c r="C59" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="63" t="s">
+      <c r="D59" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="66"/>
-      <c r="F59" s="66"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="66"/>
-      <c r="I59" s="66"/>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
-      <c r="L59" s="66"/>
-      <c r="M59" s="66"/>
-      <c r="N59" s="66"/>
-      <c r="O59" s="66"/>
-      <c r="P59" s="66"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="52"/>
+      <c r="N59" s="52"/>
+      <c r="O59" s="52"/>
+      <c r="P59" s="52"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
@@ -6126,21 +6057,21 @@
       <c r="C60" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="63" t="s">
+      <c r="D60" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="66"/>
-      <c r="F60" s="66"/>
-      <c r="G60" s="66"/>
-      <c r="H60" s="66"/>
-      <c r="I60" s="66"/>
-      <c r="J60" s="66"/>
-      <c r="K60" s="66"/>
-      <c r="L60" s="66"/>
-      <c r="M60" s="66"/>
-      <c r="N60" s="66"/>
-      <c r="O60" s="66"/>
-      <c r="P60" s="66"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="52"/>
+      <c r="L60" s="52"/>
+      <c r="M60" s="52"/>
+      <c r="N60" s="52"/>
+      <c r="O60" s="52"/>
+      <c r="P60" s="52"/>
     </row>
     <row r="61" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
@@ -6150,21 +6081,21 @@
       <c r="C61" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="65" t="s">
+      <c r="D61" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="E61" s="67"/>
-      <c r="F61" s="67"/>
-      <c r="G61" s="67"/>
-      <c r="H61" s="67"/>
-      <c r="I61" s="67"/>
-      <c r="J61" s="67"/>
-      <c r="K61" s="67"/>
-      <c r="L61" s="67"/>
-      <c r="M61" s="67"/>
-      <c r="N61" s="67"/>
-      <c r="O61" s="67"/>
-      <c r="P61" s="67"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="54"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="54"/>
+      <c r="L61" s="54"/>
+      <c r="M61" s="54"/>
+      <c r="N61" s="54"/>
+      <c r="O61" s="54"/>
+      <c r="P61" s="54"/>
     </row>
     <row r="62" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
@@ -6174,21 +6105,21 @@
       <c r="C62" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="63" t="s">
+      <c r="D62" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E62" s="66"/>
-      <c r="F62" s="66"/>
-      <c r="G62" s="66"/>
-      <c r="H62" s="66"/>
-      <c r="I62" s="66"/>
-      <c r="J62" s="66"/>
-      <c r="K62" s="66"/>
-      <c r="L62" s="66"/>
-      <c r="M62" s="66"/>
-      <c r="N62" s="66"/>
-      <c r="O62" s="66"/>
-      <c r="P62" s="66"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="52"/>
+      <c r="N62" s="52"/>
+      <c r="O62" s="52"/>
+      <c r="P62" s="52"/>
     </row>
     <row r="63" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
@@ -6198,21 +6129,21 @@
       <c r="C63" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D63" s="63" t="s">
+      <c r="D63" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="E63" s="66"/>
-      <c r="F63" s="66"/>
-      <c r="G63" s="66"/>
-      <c r="H63" s="66"/>
-      <c r="I63" s="66"/>
-      <c r="J63" s="66"/>
-      <c r="K63" s="66"/>
-      <c r="L63" s="66"/>
-      <c r="M63" s="66"/>
-      <c r="N63" s="66"/>
-      <c r="O63" s="66"/>
-      <c r="P63" s="66"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="52"/>
+      <c r="O63" s="52"/>
+      <c r="P63" s="52"/>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
@@ -6233,21 +6164,21 @@
       <c r="C64" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="63" t="s">
+      <c r="D64" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="66"/>
-      <c r="F64" s="66"/>
-      <c r="G64" s="66"/>
-      <c r="H64" s="66"/>
-      <c r="I64" s="66"/>
-      <c r="J64" s="66"/>
-      <c r="K64" s="66"/>
-      <c r="L64" s="66"/>
-      <c r="M64" s="66"/>
-      <c r="N64" s="66"/>
-      <c r="O64" s="66"/>
-      <c r="P64" s="66"/>
+      <c r="E64" s="52"/>
+      <c r="F64" s="52"/>
+      <c r="G64" s="52"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="52"/>
+      <c r="K64" s="52"/>
+      <c r="L64" s="52"/>
+      <c r="M64" s="52"/>
+      <c r="N64" s="52"/>
+      <c r="O64" s="52"/>
+      <c r="P64" s="52"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
@@ -6268,21 +6199,21 @@
       <c r="C65" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="63" t="s">
+      <c r="D65" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="E65" s="66"/>
-      <c r="F65" s="66"/>
-      <c r="G65" s="66"/>
-      <c r="H65" s="66"/>
-      <c r="I65" s="66"/>
-      <c r="J65" s="66"/>
-      <c r="K65" s="66"/>
-      <c r="L65" s="66"/>
-      <c r="M65" s="66"/>
-      <c r="N65" s="66"/>
-      <c r="O65" s="66"/>
-      <c r="P65" s="66"/>
+      <c r="E65" s="52"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
+      <c r="N65" s="52"/>
+      <c r="O65" s="52"/>
+      <c r="P65" s="52"/>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
@@ -6303,21 +6234,21 @@
       <c r="C66" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D66" s="63" t="s">
+      <c r="D66" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="64"/>
-      <c r="F66" s="64"/>
-      <c r="G66" s="64"/>
-      <c r="H66" s="64"/>
-      <c r="I66" s="64"/>
-      <c r="J66" s="64"/>
-      <c r="K66" s="64"/>
-      <c r="L66" s="64"/>
-      <c r="M66" s="64"/>
-      <c r="N66" s="64"/>
-      <c r="O66" s="64"/>
-      <c r="P66" s="64"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="55"/>
+      <c r="I66" s="55"/>
+      <c r="J66" s="55"/>
+      <c r="K66" s="55"/>
+      <c r="L66" s="55"/>
+      <c r="M66" s="55"/>
+      <c r="N66" s="55"/>
+      <c r="O66" s="55"/>
+      <c r="P66" s="55"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
@@ -6338,21 +6269,21 @@
       <c r="C67" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="63" t="s">
+      <c r="D67" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="64"/>
-      <c r="F67" s="64"/>
-      <c r="G67" s="64"/>
-      <c r="H67" s="64"/>
-      <c r="I67" s="64"/>
-      <c r="J67" s="64"/>
-      <c r="K67" s="64"/>
-      <c r="L67" s="64"/>
-      <c r="M67" s="64"/>
-      <c r="N67" s="64"/>
-      <c r="O67" s="64"/>
-      <c r="P67" s="64"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
+      <c r="I67" s="55"/>
+      <c r="J67" s="55"/>
+      <c r="K67" s="55"/>
+      <c r="L67" s="55"/>
+      <c r="M67" s="55"/>
+      <c r="N67" s="55"/>
+      <c r="O67" s="55"/>
+      <c r="P67" s="55"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
@@ -33159,6 +33090,22 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C14:Z14"/>
+    <mergeCell ref="AA15:AA19"/>
+    <mergeCell ref="AA23:AA27"/>
+    <mergeCell ref="C22:Z22"/>
+    <mergeCell ref="D67:P67"/>
+    <mergeCell ref="D66:P66"/>
+    <mergeCell ref="D58:P58"/>
+    <mergeCell ref="C6:Z6"/>
+    <mergeCell ref="AA7:AA11"/>
+    <mergeCell ref="C30:Z30"/>
+    <mergeCell ref="AA31:AA35"/>
+    <mergeCell ref="C38:Z38"/>
+    <mergeCell ref="AA39:AA43"/>
+    <mergeCell ref="C46:Z46"/>
+    <mergeCell ref="AA47:AA51"/>
     <mergeCell ref="D59:P59"/>
     <mergeCell ref="D61:P61"/>
     <mergeCell ref="D64:P64"/>
@@ -33166,22 +33113,6 @@
     <mergeCell ref="D63:P63"/>
     <mergeCell ref="D62:P62"/>
     <mergeCell ref="D60:P60"/>
-    <mergeCell ref="D67:P67"/>
-    <mergeCell ref="D66:P66"/>
-    <mergeCell ref="D58:P58"/>
-    <mergeCell ref="C6:Z6"/>
-    <mergeCell ref="AA7:AA11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C14:Z14"/>
-    <mergeCell ref="AA15:AA19"/>
-    <mergeCell ref="AA23:AA27"/>
-    <mergeCell ref="C22:Z22"/>
-    <mergeCell ref="C30:Z30"/>
-    <mergeCell ref="AA31:AA35"/>
-    <mergeCell ref="C38:Z38"/>
-    <mergeCell ref="AA39:AA43"/>
-    <mergeCell ref="C46:Z46"/>
-    <mergeCell ref="AA47:AA51"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.51181102362204722" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>